<commit_message>
fix: psychopy should work in this folder
</commit_message>
<xml_diff>
--- a/conditions/mTBI_runs.xlsx
+++ b/conditions/mTBI_runs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>run_num</t>
   </si>
@@ -28,19 +28,22 @@
     <t>FB</t>
   </si>
   <si>
-    <t>mTBIconditions2.xlsx</t>
-  </si>
-  <si>
-    <t>mTBIconditions3.xlsx</t>
-  </si>
-  <si>
-    <t>mTBIconditions4.xlsx</t>
-  </si>
-  <si>
-    <t>mTBIconditions5.xlsx</t>
-  </si>
-  <si>
-    <t>mTBIconditions6.xlsx</t>
+    <t>conditions/mTBIconditions1.xlsx</t>
+  </si>
+  <si>
+    <t>conditions/mTBIconditions2.xlsx</t>
+  </si>
+  <si>
+    <t>conditions/mTBIconditions3.xlsx</t>
+  </si>
+  <si>
+    <t>conditions/mTBIconditions4.xlsx</t>
+  </si>
+  <si>
+    <t>conditions/mTBIconditions5.xlsx</t>
+  </si>
+  <si>
+    <t>conditions/mTBIconditions6.xlsx</t>
   </si>
 </sst>
 </file>
@@ -134,16 +137,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="B7" activeCellId="0" pane="topLeft" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -159,18 +162,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
@@ -181,7 +184,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>5</v>
@@ -192,7 +195,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
@@ -203,12 +206,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -231,11 +245,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B7 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -256,11 +270,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B7 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>